<commit_message>
scripts acabados, excel hechos y tal
</commit_message>
<xml_diff>
--- a/PROJECT/PreciosValoracionesAirbnb/Excel Salidas/Barcelona/averagePriceBarcelonaNeighbourhoods.xlsx
+++ b/PROJECT/PreciosValoracionesAirbnb/Excel Salidas/Barcelona/averagePriceBarcelonaNeighbourhoods.xlsx
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>neighbourhood_cleansed</t>
+          <t>neighbourhood</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -448,311 +448,311 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>el Poblenou</t>
+          <t>Baró de Viver</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>87.63786008230453</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>el Besòs i el Maresme</t>
+          <t>Can Peguera</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>58.98584905660378</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>la Vila de Gràcia</t>
+          <t>la Trinitat Nova</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>109.8095238095238</v>
+        <v>28.7</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>la Guineueta</t>
+          <t>Montbau</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>57</v>
+        <v>29.1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>la Teixonera</t>
+          <t>Verdun</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>47.5945945945946</v>
+        <v>32.96551724137931</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>la Dreta de l'Eixample</t>
+          <t>Ciutat Meridiana</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>157.3862851504687</v>
+        <v>34.14285714285715</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>el Barri Gòtic</t>
+          <t>la Prosperitat</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>84.39941262848753</v>
+        <v>37.42105263157895</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>el Guinardó</t>
+          <t>Torre Baró</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>72.54589371980677</v>
+        <v>39.5</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Canyelles</t>
+          <t>el Congrés i els Indians</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>43.5</v>
+        <v>40.15714285714286</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Provençals del Poblenou</t>
+          <t>les Roquetes</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>68.96747967479675</v>
+        <v>41.09677419354838</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>la Verneda i la Pau</t>
+          <t>Horta</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>42.8235294117647</v>
+        <v>41.68292682926829</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Vilapicina i la Torre Llobeta</t>
+          <t>la Verneda i la Pau</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>53.94</v>
+        <v>42.8235294117647</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>l'Antiga Esquerra de l'Eixample</t>
+          <t>la Sagrera</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>107.5867393278837</v>
+        <v>43.40243902439025</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Navas</t>
+          <t>Canyelles</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>45.96</v>
+        <v>43.5</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>la Marina de Port</t>
+          <t>la Font d'en Fargues</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>63.93548387096774</v>
+        <v>44.47619047619047</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Sarrià</t>
+          <t>la Trinitat Vella</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>86.97297297297297</v>
+        <v>45.3125</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>la Marina del Prat Vermell</t>
+          <t>Sant Martí de Provençals</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>98</v>
+        <v>45.49473684210526</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Torre Baró</t>
+          <t>la Vall d'Hebron</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>39.5</v>
+        <v>45.81818181818182</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Sant Antoni</t>
+          <t>Navas</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>92.06593406593407</v>
+        <v>45.96</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Sant Gervasi - Galvany</t>
+          <t>el Bon Pastor</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>110.4210526315789</v>
+        <v>46.08</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>les Roquetes</t>
+          <t>la Teixonera</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>41.09677419354838</v>
+        <v>47.5945945945946</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>el Congrés i els Indians</t>
+          <t>Porta</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>40.15714285714286</v>
+        <v>48.5</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Sant Pere, Santa Caterina i la Ribera</t>
+          <t>el Turó de la Peira</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>84.22355769230769</v>
+        <v>49.25806451612903</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>la Vall d'Hebron</t>
+          <t>Sant Andreu</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>45.81818181818182</v>
+        <v>52.04225352112676</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>el Bon Pastor</t>
+          <t>Vilapicina i la Torre Llobeta</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>46.08</v>
+        <v>53.94</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Sants - Badal</t>
+          <t>el Coll</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>60.21390374331551</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>la Nova Esquerra de l'Eixample</t>
+          <t>la Guineueta</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>79.63403781979977</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Can Baró</t>
+          <t>la Maternitat i Sant Ramon</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>72.32558139534883</v>
+        <v>58.01785714285715</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>les Corts</t>
+          <t>el Besòs i el Maresme</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>89.39583333333333</v>
+        <v>58.98584905660378</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>la Sagrera</t>
+          <t>la Bordeta</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>43.40243902439025</v>
+        <v>59.4718309859155</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Verdun</t>
+          <t>Sants - Badal</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>32.96551724137931</v>
+        <v>60.21390374331551</v>
       </c>
     </row>
     <row r="33">
@@ -768,11 +768,11 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>el Camp d'en Grassot i Gràcia Nova</t>
+          <t>la Marina de Port</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>80.70977011494253</v>
+        <v>63.93548387096774</v>
       </c>
     </row>
     <row r="35">
@@ -798,361 +798,361 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>el Poble Sec</t>
+          <t>Sant Gervasi - la Bonanova</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>82.49063336306868</v>
+        <v>66.57142857142857</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Sant Gervasi - la Bonanova</t>
+          <t>la Salut</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>66.57142857142857</v>
+        <v>67.34545454545454</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Porta</t>
+          <t>Provençals del Poblenou</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>48.5</v>
+        <v>68.96747967479675</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Horta</t>
+          <t>el Camp de l'Arpa del Clot</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>41.68292682926829</v>
+        <v>71.57386363636364</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>el Camp de l'Arpa del Clot</t>
+          <t>Can Baró</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>71.57386363636364</v>
+        <v>72.32558139534883</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Diagonal Mar i el Front Marítim del Poblenou</t>
+          <t>Sant Genís dels Agudells</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>174.139896373057</v>
+        <v>72.375</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>la Maternitat i Sant Ramon</t>
+          <t>el Guinardó</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>58.01785714285715</v>
+        <v>72.54589371980677</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>el Parc i la Llacuna del Poblenou</t>
+          <t>la Barceloneta</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>76.11481481481482</v>
+        <v>73.07877461706784</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>el Carmel</t>
+          <t>el Raval</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>98.40000000000001</v>
+        <v>74.72722095671982</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>la Prosperitat</t>
+          <t>el Parc i la Llacuna del Poblenou</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>37.42105263157895</v>
+        <v>76.11481481481482</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>el Fort Pienc</t>
+          <t>Sants</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>107.992380952381</v>
+        <v>76.97323600973236</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>el Putxet i el Farró</t>
+          <t>la Nova Esquerra de l'Eixample</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>105.4778761061947</v>
+        <v>79.63403781979977</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Sant Andreu</t>
+          <t>Vallcarca i els Penitents</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>52.04225352112676</v>
+        <v>80.09917355371901</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>les Tres Torres</t>
+          <t>el Camp d'en Grassot i Gràcia Nova</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>106.8333333333333</v>
+        <v>80.70977011494253</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>la Bordeta</t>
+          <t>el Poble Sec</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>59.4718309859155</v>
+        <v>82.49063336306868</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>el Coll</t>
+          <t>Sant Pere, Santa Caterina i la Ribera</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>54</v>
+        <v>84.22355769230769</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>el Turó de la Peira</t>
+          <t>el Barri Gòtic</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>49.25806451612903</v>
+        <v>84.39941262848753</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>la Font d'en Fargues</t>
+          <t>Sarrià</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>44.47619047619047</v>
+        <v>86.97297297297297</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Hostafrancs</t>
+          <t>el Poblenou</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>94.93220338983051</v>
+        <v>87.63786008230453</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Montbau</t>
+          <t>les Corts</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>29.1</v>
+        <v>89.39583333333333</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Pedralbes</t>
+          <t>Sant Antoni</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>97.23076923076923</v>
+        <v>92.06593406593407</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Sant Martí de Provençals</t>
+          <t>Hostafrancs</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>45.49473684210526</v>
+        <v>94.93220338983051</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Vallcarca i els Penitents</t>
+          <t>Pedralbes</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>80.09917355371901</v>
+        <v>97.23076923076923</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>el Raval</t>
+          <t>la Sagrada Família</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>74.72722095671982</v>
+        <v>97.2675799086758</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Sants</t>
+          <t>la Marina del Prat Vermell</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>76.97323600973236</v>
+        <v>98</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Vallvidrera, el Tibidabo i les Planes</t>
+          <t>el Carmel</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>125.9677419354839</v>
+        <v>98.40000000000001</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Ciutat Meridiana</t>
+          <t>el Putxet i el Farró</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>34.14285714285715</v>
+        <v>105.4778761061947</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>la Barceloneta</t>
+          <t>les Tres Torres</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>73.07877461706784</v>
+        <v>106.8333333333333</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>la Salut</t>
+          <t>l'Antiga Esquerra de l'Eixample</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>67.34545454545454</v>
+        <v>107.5867393278837</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Sant Genís dels Agudells</t>
+          <t>el Fort Pienc</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>72.375</v>
+        <v>107.992380952381</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>la Vila Olímpica del Poblenou</t>
+          <t>la Vila de Gràcia</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>170.3422459893048</v>
+        <v>109.8095238095238</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>la Sagrada Família</t>
+          <t>Sant Gervasi - Galvany</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>97.2675799086758</v>
+        <v>110.4210526315789</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>la Trinitat Nova</t>
+          <t>Vallvidrera, el Tibidabo i les Planes</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>28.7</v>
+        <v>125.9677419354839</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>la Trinitat Vella</t>
+          <t>la Dreta de l'Eixample</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>45.3125</v>
+        <v>157.3862851504687</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Baró de Viver</t>
+          <t>la Vila Olímpica del Poblenou</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>21.5</v>
+        <v>170.3422459893048</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Can Peguera</t>
+          <t>Diagonal Mar i el Front Marítim del Poblenou</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>25</v>
+        <v>174.139896373057</v>
       </c>
     </row>
   </sheetData>

</xml_diff>